<commit_message>
Hunt Team Heat Map Update
</commit_message>
<xml_diff>
--- a/metrics/HuntTeam_HeatMap.xlsx
+++ b/metrics/HuntTeam_HeatMap.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wardog\Documents\MITRE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HIVE\github\ThreatHunter-Playbook\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="HeatMap" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="Trends" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1293" uniqueCount="674">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1293" uniqueCount="673">
   <si>
     <t>Persistence</t>
   </si>
@@ -1090,11 +1089,6 @@
   </si>
   <si>
     <t>File monitoring, Process monitoring, Process use of network</t>
-  </si>
-  <si>
-    <t>PR
-Moloch
-Niksun</t>
   </si>
   <si>
     <t>The BIOS (Basic Input/Output System), which underlies the functionality of a computer, may be modified to perform or assist in malicious activity.
@@ -2617,7 +2611,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2729,7 +2722,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2884,7 +2876,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3039,7 +3030,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3194,7 +3184,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3349,7 +3338,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3504,7 +3492,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3661,7 +3648,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3818,7 +3804,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3975,7 +3960,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -4132,7 +4116,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -4226,11 +4209,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1720296320"/>
-        <c:axId val="1720283264"/>
+        <c:axId val="1881331744"/>
+        <c:axId val="1881311616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1720296320"/>
+        <c:axId val="1881331744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4272,7 +4255,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1720283264"/>
+        <c:crossAx val="1881311616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4280,7 +4263,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1720283264"/>
+        <c:axId val="1881311616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4330,7 +4313,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1720296320"/>
+        <c:crossAx val="1881331744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4344,7 +4327,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5258,7 +5240,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
@@ -7092,8 +7074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H139"/>
   <sheetViews>
-    <sheetView topLeftCell="A132" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B111" sqref="B111"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7157,7 +7139,7 @@
         <v>149</v>
       </c>
       <c r="H2" s="30" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="120" x14ac:dyDescent="0.25">
@@ -7183,7 +7165,7 @@
         <v>148</v>
       </c>
       <c r="H3" s="30" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="135" x14ac:dyDescent="0.25">
@@ -7203,13 +7185,13 @@
         <v>343</v>
       </c>
       <c r="F4" s="30" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="G4" s="30" t="s">
         <v>149</v>
       </c>
       <c r="H4" s="30" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="135" x14ac:dyDescent="0.25">
@@ -7235,7 +7217,7 @@
         <v>148</v>
       </c>
       <c r="H5" s="30" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="149.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7261,7 +7243,7 @@
         <v>147</v>
       </c>
       <c r="H6" s="30" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="150" x14ac:dyDescent="0.25">
@@ -7287,7 +7269,7 @@
         <v>147</v>
       </c>
       <c r="H7" s="30" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7313,7 +7295,7 @@
         <v>149</v>
       </c>
       <c r="H8" s="22" t="s">
-        <v>353</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="132.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7327,13 +7309,13 @@
         <v>187</v>
       </c>
       <c r="D9" s="30" t="s">
+        <v>353</v>
+      </c>
+      <c r="E9" s="30" t="s">
         <v>354</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="F9" s="30" t="s">
         <v>355</v>
-      </c>
-      <c r="F9" s="30" t="s">
-        <v>356</v>
       </c>
       <c r="G9" s="30" t="s">
         <v>147</v>
@@ -7356,10 +7338,10 @@
         <v>175</v>
       </c>
       <c r="E10" s="30" t="s">
+        <v>356</v>
+      </c>
+      <c r="F10" s="30" t="s">
         <v>357</v>
-      </c>
-      <c r="F10" s="30" t="s">
-        <v>358</v>
       </c>
       <c r="G10" s="30" t="s">
         <v>148</v>
@@ -7379,13 +7361,13 @@
         <v>253</v>
       </c>
       <c r="D11" s="30" t="s">
+        <v>358</v>
+      </c>
+      <c r="E11" s="30" t="s">
         <v>359</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="F11" s="30" t="s">
         <v>360</v>
-      </c>
-      <c r="F11" s="30" t="s">
-        <v>361</v>
       </c>
       <c r="G11" s="30" t="s">
         <v>147</v>
@@ -7405,13 +7387,13 @@
         <v>308</v>
       </c>
       <c r="D12" s="30" t="s">
+        <v>361</v>
+      </c>
+      <c r="E12" s="30" t="s">
         <v>362</v>
       </c>
-      <c r="E12" s="30" t="s">
+      <c r="F12" s="30" t="s">
         <v>363</v>
-      </c>
-      <c r="F12" s="30" t="s">
-        <v>364</v>
       </c>
       <c r="G12" s="30" t="s">
         <v>149</v>
@@ -7425,19 +7407,19 @@
         <v>20</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C13" s="26" t="s">
         <v>279</v>
       </c>
       <c r="D13" s="30" t="s">
+        <v>365</v>
+      </c>
+      <c r="E13" s="30" t="s">
         <v>366</v>
       </c>
-      <c r="E13" s="30" t="s">
+      <c r="F13" s="30" t="s">
         <v>367</v>
-      </c>
-      <c r="F13" s="30" t="s">
-        <v>368</v>
       </c>
       <c r="G13" s="30" t="s">
         <v>147</v>
@@ -7457,13 +7439,13 @@
         <v>219</v>
       </c>
       <c r="D14" s="30" t="s">
+        <v>368</v>
+      </c>
+      <c r="E14" s="30" t="s">
         <v>369</v>
       </c>
-      <c r="E14" s="30" t="s">
+      <c r="F14" s="30" t="s">
         <v>370</v>
-      </c>
-      <c r="F14" s="30" t="s">
-        <v>371</v>
       </c>
       <c r="G14" s="30" t="s">
         <v>147</v>
@@ -7483,13 +7465,13 @@
         <v>314</v>
       </c>
       <c r="D15" s="30" t="s">
+        <v>371</v>
+      </c>
+      <c r="E15" s="30" t="s">
         <v>372</v>
       </c>
-      <c r="E15" s="30" t="s">
+      <c r="F15" s="30" t="s">
         <v>373</v>
-      </c>
-      <c r="F15" s="30" t="s">
-        <v>374</v>
       </c>
       <c r="G15" s="30" t="s">
         <v>147</v>
@@ -7509,13 +7491,13 @@
         <v>315</v>
       </c>
       <c r="D16" s="30" t="s">
+        <v>374</v>
+      </c>
+      <c r="E16" s="30" t="s">
         <v>375</v>
       </c>
-      <c r="E16" s="30" t="s">
+      <c r="F16" s="30" t="s">
         <v>376</v>
-      </c>
-      <c r="F16" s="30" t="s">
-        <v>377</v>
       </c>
       <c r="G16" s="30" t="s">
         <v>147</v>
@@ -7535,13 +7517,13 @@
         <v>242</v>
       </c>
       <c r="D17" s="30" t="s">
+        <v>377</v>
+      </c>
+      <c r="E17" s="30" t="s">
         <v>378</v>
       </c>
-      <c r="E17" s="30" t="s">
+      <c r="F17" s="30" t="s">
         <v>379</v>
-      </c>
-      <c r="F17" s="30" t="s">
-        <v>380</v>
       </c>
       <c r="G17" s="30" t="s">
         <v>147</v>
@@ -7561,13 +7543,13 @@
         <v>220</v>
       </c>
       <c r="D18" s="30" t="s">
+        <v>380</v>
+      </c>
+      <c r="E18" s="30" t="s">
         <v>381</v>
       </c>
-      <c r="E18" s="30" t="s">
+      <c r="F18" s="30" t="s">
         <v>382</v>
-      </c>
-      <c r="F18" s="30" t="s">
-        <v>383</v>
       </c>
       <c r="G18" s="30" t="s">
         <v>148</v>
@@ -7590,10 +7572,10 @@
         <v>286</v>
       </c>
       <c r="E19" s="30" t="s">
+        <v>383</v>
+      </c>
+      <c r="F19" s="30" t="s">
         <v>384</v>
-      </c>
-      <c r="F19" s="30" t="s">
-        <v>385</v>
       </c>
       <c r="G19" s="30" t="s">
         <v>148</v>
@@ -7607,7 +7589,7 @@
         <v>39</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C20" s="26" t="s">
         <v>306</v>
@@ -7629,19 +7611,19 @@
         <v>49</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C21" s="26" t="s">
         <v>322</v>
       </c>
       <c r="D21" s="30" t="s">
+        <v>386</v>
+      </c>
+      <c r="E21" s="30" t="s">
         <v>387</v>
       </c>
-      <c r="E21" s="30" t="s">
+      <c r="F21" s="30" t="s">
         <v>388</v>
-      </c>
-      <c r="F21" s="30" t="s">
-        <v>389</v>
       </c>
       <c r="G21" s="30" t="s">
         <v>147</v>
@@ -7661,13 +7643,13 @@
         <v>282</v>
       </c>
       <c r="D22" s="30" t="s">
+        <v>389</v>
+      </c>
+      <c r="E22" s="30" t="s">
         <v>390</v>
       </c>
-      <c r="E22" s="30" t="s">
+      <c r="F22" s="30" t="s">
         <v>391</v>
-      </c>
-      <c r="F22" s="30" t="s">
-        <v>392</v>
       </c>
       <c r="G22" s="30" t="s">
         <v>148</v>
@@ -7687,13 +7669,13 @@
         <v>166</v>
       </c>
       <c r="D23" s="30" t="s">
+        <v>392</v>
+      </c>
+      <c r="E23" s="30" t="s">
         <v>393</v>
       </c>
-      <c r="E23" s="30" t="s">
+      <c r="F23" s="30" t="s">
         <v>394</v>
-      </c>
-      <c r="F23" s="30" t="s">
-        <v>395</v>
       </c>
       <c r="G23" s="30" t="s">
         <v>149</v>
@@ -7716,10 +7698,10 @@
         <v>294</v>
       </c>
       <c r="E24" s="30" t="s">
+        <v>395</v>
+      </c>
+      <c r="F24" s="30" t="s">
         <v>396</v>
-      </c>
-      <c r="F24" s="30" t="s">
-        <v>397</v>
       </c>
       <c r="G24" s="30" t="s">
         <v>149</v>
@@ -7739,13 +7721,13 @@
         <v>272</v>
       </c>
       <c r="D25" s="30" t="s">
+        <v>397</v>
+      </c>
+      <c r="E25" s="30" t="s">
         <v>398</v>
       </c>
-      <c r="E25" s="30" t="s">
+      <c r="F25" s="30" t="s">
         <v>399</v>
-      </c>
-      <c r="F25" s="30" t="s">
-        <v>400</v>
       </c>
       <c r="G25" s="30" t="s">
         <v>148</v>
@@ -7768,10 +7750,10 @@
         <v>289</v>
       </c>
       <c r="E26" s="30" t="s">
+        <v>381</v>
+      </c>
+      <c r="F26" s="30" t="s">
         <v>382</v>
-      </c>
-      <c r="F26" s="30" t="s">
-        <v>383</v>
       </c>
       <c r="G26" s="30" t="s">
         <v>149</v>
@@ -7791,13 +7773,13 @@
         <v>194</v>
       </c>
       <c r="D27" s="30" t="s">
+        <v>400</v>
+      </c>
+      <c r="E27" s="30" t="s">
         <v>401</v>
       </c>
-      <c r="E27" s="30" t="s">
+      <c r="F27" s="30" t="s">
         <v>402</v>
-      </c>
-      <c r="F27" s="30" t="s">
-        <v>403</v>
       </c>
       <c r="G27" s="30" t="s">
         <v>148</v>
@@ -7820,10 +7802,10 @@
         <v>165</v>
       </c>
       <c r="E28" s="30" t="s">
+        <v>403</v>
+      </c>
+      <c r="F28" s="30" t="s">
         <v>404</v>
-      </c>
-      <c r="F28" s="30" t="s">
-        <v>405</v>
       </c>
       <c r="G28" s="30" t="s">
         <v>148</v>
@@ -7843,13 +7825,13 @@
         <v>191</v>
       </c>
       <c r="D29" s="30" t="s">
+        <v>405</v>
+      </c>
+      <c r="E29" s="30" t="s">
         <v>406</v>
       </c>
-      <c r="E29" s="30" t="s">
+      <c r="F29" s="30" t="s">
         <v>407</v>
-      </c>
-      <c r="F29" s="30" t="s">
-        <v>408</v>
       </c>
       <c r="G29" s="30" t="s">
         <v>148</v>
@@ -7869,13 +7851,13 @@
         <v>169</v>
       </c>
       <c r="D30" s="30" t="s">
+        <v>408</v>
+      </c>
+      <c r="E30" s="30" t="s">
         <v>409</v>
       </c>
-      <c r="E30" s="30" t="s">
+      <c r="F30" s="30" t="s">
         <v>410</v>
-      </c>
-      <c r="F30" s="30" t="s">
-        <v>411</v>
       </c>
       <c r="G30" s="30" t="s">
         <v>147</v>
@@ -7895,13 +7877,13 @@
         <v>214</v>
       </c>
       <c r="D31" s="30" t="s">
+        <v>411</v>
+      </c>
+      <c r="E31" s="30" t="s">
         <v>412</v>
       </c>
-      <c r="E31" s="30" t="s">
-        <v>413</v>
-      </c>
       <c r="F31" s="30" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G31" s="30" t="s">
         <v>147</v>
@@ -7921,13 +7903,13 @@
         <v>195</v>
       </c>
       <c r="D32" s="30" t="s">
+        <v>413</v>
+      </c>
+      <c r="E32" s="30" t="s">
         <v>414</v>
       </c>
-      <c r="E32" s="30" t="s">
-        <v>415</v>
-      </c>
       <c r="F32" s="30" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G32" s="30" t="s">
         <v>147</v>
@@ -7947,13 +7929,13 @@
         <v>163</v>
       </c>
       <c r="D33" s="30" t="s">
+        <v>415</v>
+      </c>
+      <c r="E33" s="22" t="s">
+        <v>381</v>
+      </c>
+      <c r="F33" s="22" t="s">
         <v>416</v>
-      </c>
-      <c r="E33" s="22" t="s">
-        <v>382</v>
-      </c>
-      <c r="F33" s="22" t="s">
-        <v>417</v>
       </c>
       <c r="G33" s="30" t="s">
         <v>149</v>
@@ -7973,13 +7955,13 @@
         <v>263</v>
       </c>
       <c r="D34" s="30" t="s">
+        <v>417</v>
+      </c>
+      <c r="E34" s="30" t="s">
         <v>418</v>
       </c>
-      <c r="E34" s="30" t="s">
-        <v>419</v>
-      </c>
       <c r="F34" s="30" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G34" s="30" t="s">
         <v>147</v>
@@ -8002,10 +7984,10 @@
         <v>204</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F35" s="30" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G35" s="30" t="s">
         <v>149</v>
@@ -8028,10 +8010,10 @@
         <v>281</v>
       </c>
       <c r="E36" s="30" t="s">
+        <v>420</v>
+      </c>
+      <c r="F36" s="30" t="s">
         <v>421</v>
-      </c>
-      <c r="F36" s="30" t="s">
-        <v>422</v>
       </c>
       <c r="G36" s="30" t="s">
         <v>148</v>
@@ -8045,19 +8027,19 @@
         <v>38</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C37" s="26" t="s">
         <v>237</v>
       </c>
       <c r="D37" s="30" t="s">
+        <v>422</v>
+      </c>
+      <c r="E37" s="30" t="s">
         <v>423</v>
       </c>
-      <c r="E37" s="30" t="s">
+      <c r="F37" s="30" t="s">
         <v>424</v>
-      </c>
-      <c r="F37" s="30" t="s">
-        <v>425</v>
       </c>
       <c r="G37" s="30" t="s">
         <v>148</v>
@@ -8071,19 +8053,19 @@
         <v>48</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C38" s="26" t="s">
         <v>213</v>
       </c>
       <c r="D38" s="30" t="s">
+        <v>426</v>
+      </c>
+      <c r="E38" s="30" t="s">
         <v>427</v>
       </c>
-      <c r="E38" s="30" t="s">
+      <c r="F38" s="30" t="s">
         <v>428</v>
-      </c>
-      <c r="F38" s="30" t="s">
-        <v>429</v>
       </c>
       <c r="G38" s="30" t="s">
         <v>148</v>
@@ -8103,13 +8085,13 @@
         <v>262</v>
       </c>
       <c r="D39" s="30" t="s">
+        <v>429</v>
+      </c>
+      <c r="E39" s="30" t="s">
         <v>430</v>
       </c>
-      <c r="E39" s="30" t="s">
+      <c r="F39" s="30" t="s">
         <v>431</v>
-      </c>
-      <c r="F39" s="30" t="s">
-        <v>432</v>
       </c>
       <c r="G39" s="30" t="s">
         <v>147</v>
@@ -8129,13 +8111,13 @@
         <v>313</v>
       </c>
       <c r="D40" s="30" t="s">
+        <v>432</v>
+      </c>
+      <c r="E40" s="30" t="s">
         <v>433</v>
       </c>
-      <c r="E40" s="30" t="s">
+      <c r="F40" s="30" t="s">
         <v>434</v>
-      </c>
-      <c r="F40" s="30" t="s">
-        <v>435</v>
       </c>
       <c r="G40" s="30" t="s">
         <v>147</v>
@@ -8155,13 +8137,13 @@
         <v>303</v>
       </c>
       <c r="D41" s="30" t="s">
+        <v>435</v>
+      </c>
+      <c r="E41" s="30" t="s">
         <v>436</v>
       </c>
-      <c r="E41" s="30" t="s">
+      <c r="F41" s="30" t="s">
         <v>437</v>
-      </c>
-      <c r="F41" s="30" t="s">
-        <v>438</v>
       </c>
       <c r="G41" s="30" t="s">
         <v>147</v>
@@ -8184,10 +8166,10 @@
         <v>227</v>
       </c>
       <c r="E42" s="30" t="s">
+        <v>438</v>
+      </c>
+      <c r="F42" s="30" t="s">
         <v>439</v>
-      </c>
-      <c r="F42" s="30" t="s">
-        <v>440</v>
       </c>
       <c r="G42" s="30" t="s">
         <v>148</v>
@@ -8210,10 +8192,10 @@
         <v>218</v>
       </c>
       <c r="E43" s="30" t="s">
+        <v>381</v>
+      </c>
+      <c r="F43" s="30" t="s">
         <v>382</v>
-      </c>
-      <c r="F43" s="30" t="s">
-        <v>383</v>
       </c>
       <c r="G43" s="30" t="s">
         <v>148</v>
@@ -8233,13 +8215,13 @@
         <v>178</v>
       </c>
       <c r="D44" s="30" t="s">
+        <v>440</v>
+      </c>
+      <c r="E44" s="30" t="s">
         <v>441</v>
       </c>
-      <c r="E44" s="30" t="s">
-        <v>442</v>
-      </c>
       <c r="F44" s="30" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="G44" s="30" t="s">
         <v>148</v>
@@ -8262,10 +8244,10 @@
         <v>233</v>
       </c>
       <c r="E45" s="30" t="s">
+        <v>442</v>
+      </c>
+      <c r="F45" s="30" t="s">
         <v>443</v>
-      </c>
-      <c r="F45" s="30" t="s">
-        <v>444</v>
       </c>
       <c r="G45" s="30" t="s">
         <v>148</v>
@@ -8279,19 +8261,19 @@
         <v>23</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C46" s="26" t="s">
         <v>254</v>
       </c>
       <c r="D46" s="30" t="s">
+        <v>445</v>
+      </c>
+      <c r="E46" s="30" t="s">
         <v>446</v>
       </c>
-      <c r="E46" s="30" t="s">
+      <c r="F46" s="30" t="s">
         <v>447</v>
-      </c>
-      <c r="F46" s="30" t="s">
-        <v>448</v>
       </c>
       <c r="G46" s="30" t="s">
         <v>148</v>
@@ -8314,10 +8296,10 @@
         <v>173</v>
       </c>
       <c r="E47" s="30" t="s">
+        <v>448</v>
+      </c>
+      <c r="F47" s="30" t="s">
         <v>449</v>
-      </c>
-      <c r="F47" s="30" t="s">
-        <v>450</v>
       </c>
       <c r="G47" s="30" t="s">
         <v>148</v>
@@ -8337,13 +8319,13 @@
         <v>274</v>
       </c>
       <c r="D48" s="30" t="s">
+        <v>450</v>
+      </c>
+      <c r="E48" s="30" t="s">
+        <v>390</v>
+      </c>
+      <c r="F48" s="30" t="s">
         <v>451</v>
-      </c>
-      <c r="E48" s="30" t="s">
-        <v>391</v>
-      </c>
-      <c r="F48" s="30" t="s">
-        <v>452</v>
       </c>
       <c r="G48" s="30" t="s">
         <v>147</v>
@@ -8363,13 +8345,13 @@
         <v>304</v>
       </c>
       <c r="D49" s="30" t="s">
+        <v>452</v>
+      </c>
+      <c r="E49" s="30" t="s">
         <v>453</v>
       </c>
-      <c r="E49" s="30" t="s">
+      <c r="F49" s="30" t="s">
         <v>454</v>
-      </c>
-      <c r="F49" s="30" t="s">
-        <v>455</v>
       </c>
       <c r="G49" s="30" t="s">
         <v>148</v>
@@ -8389,13 +8371,13 @@
         <v>170</v>
       </c>
       <c r="D50" s="30" t="s">
+        <v>455</v>
+      </c>
+      <c r="E50" s="30" t="s">
         <v>456</v>
       </c>
-      <c r="E50" s="30" t="s">
+      <c r="F50" s="30" t="s">
         <v>457</v>
-      </c>
-      <c r="F50" s="30" t="s">
-        <v>458</v>
       </c>
       <c r="G50" s="30" t="s">
         <v>147</v>
@@ -8418,10 +8400,10 @@
         <v>245</v>
       </c>
       <c r="E51" s="30" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F51" s="30" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="G51" s="30" t="s">
         <v>147</v>
@@ -8441,13 +8423,13 @@
         <v>246</v>
       </c>
       <c r="D52" s="30" t="s">
+        <v>459</v>
+      </c>
+      <c r="E52" s="30" t="s">
         <v>460</v>
       </c>
-      <c r="E52" s="30" t="s">
+      <c r="F52" s="30" t="s">
         <v>461</v>
-      </c>
-      <c r="F52" s="30" t="s">
-        <v>462</v>
       </c>
       <c r="G52" s="30" t="s">
         <v>147</v>
@@ -8470,10 +8452,10 @@
         <v>236</v>
       </c>
       <c r="E53" s="30" t="s">
+        <v>462</v>
+      </c>
+      <c r="F53" s="30" t="s">
         <v>463</v>
-      </c>
-      <c r="F53" s="30" t="s">
-        <v>464</v>
       </c>
       <c r="G53" s="30" t="s">
         <v>147</v>
@@ -8496,10 +8478,10 @@
         <v>252</v>
       </c>
       <c r="E54" s="30" t="s">
+        <v>465</v>
+      </c>
+      <c r="F54" s="30" t="s">
         <v>466</v>
-      </c>
-      <c r="F54" s="30" t="s">
-        <v>467</v>
       </c>
       <c r="G54" s="30" t="s">
         <v>148</v>
@@ -8522,10 +8504,10 @@
         <v>258</v>
       </c>
       <c r="E55" s="30" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F55" s="30" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G55" s="30" t="s">
         <v>148</v>
@@ -8539,19 +8521,19 @@
         <v>57</v>
       </c>
       <c r="B56" s="21" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C56" s="26" t="s">
         <v>238</v>
       </c>
       <c r="D56" s="30" t="s">
+        <v>469</v>
+      </c>
+      <c r="E56" s="30" t="s">
         <v>470</v>
       </c>
-      <c r="E56" s="30" t="s">
+      <c r="F56" s="30" t="s">
         <v>471</v>
-      </c>
-      <c r="F56" s="30" t="s">
-        <v>472</v>
       </c>
       <c r="G56" s="30" t="s">
         <v>147</v>
@@ -8565,19 +8547,19 @@
         <v>52</v>
       </c>
       <c r="B57" s="21" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C57" s="26" t="s">
         <v>317</v>
       </c>
       <c r="D57" s="30" t="s">
+        <v>473</v>
+      </c>
+      <c r="E57" s="30" t="s">
         <v>474</v>
       </c>
-      <c r="E57" s="30" t="s">
+      <c r="F57" s="30" t="s">
         <v>475</v>
-      </c>
-      <c r="F57" s="30" t="s">
-        <v>476</v>
       </c>
       <c r="G57" s="30" t="s">
         <v>150</v>
@@ -8591,19 +8573,19 @@
         <v>72</v>
       </c>
       <c r="B58" s="21" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C58" s="26" t="s">
         <v>267</v>
       </c>
       <c r="D58" s="30" t="s">
+        <v>477</v>
+      </c>
+      <c r="E58" s="30" t="s">
         <v>478</v>
       </c>
-      <c r="E58" s="30" t="s">
+      <c r="F58" s="30" t="s">
         <v>479</v>
-      </c>
-      <c r="F58" s="30" t="s">
-        <v>480</v>
       </c>
       <c r="G58" s="30" t="s">
         <v>148</v>
@@ -8623,13 +8605,13 @@
         <v>183</v>
       </c>
       <c r="D59" s="30" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E59" s="31" t="s">
         <v>346</v>
       </c>
       <c r="F59" s="30" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G59" s="30" t="s">
         <v>147</v>
@@ -8649,16 +8631,16 @@
         <v>228</v>
       </c>
       <c r="D60" s="30" t="s">
+        <v>481</v>
+      </c>
+      <c r="E60" s="30" t="s">
+        <v>390</v>
+      </c>
+      <c r="F60" s="30" t="s">
         <v>482</v>
       </c>
-      <c r="E60" s="30" t="s">
-        <v>391</v>
-      </c>
-      <c r="F60" s="30" t="s">
-        <v>483</v>
-      </c>
       <c r="G60" s="30" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="H60" s="30" t="s">
         <v>147</v>
@@ -8675,13 +8657,13 @@
         <v>180</v>
       </c>
       <c r="D61" s="30" t="s">
+        <v>483</v>
+      </c>
+      <c r="E61" s="30" t="s">
         <v>484</v>
       </c>
-      <c r="E61" s="30" t="s">
+      <c r="F61" s="30" t="s">
         <v>485</v>
-      </c>
-      <c r="F61" s="30" t="s">
-        <v>486</v>
       </c>
       <c r="G61" s="30" t="s">
         <v>149</v>
@@ -8695,19 +8677,19 @@
         <v>32</v>
       </c>
       <c r="B62" s="21" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C62" s="26" t="s">
         <v>212</v>
       </c>
       <c r="D62" s="30" t="s">
+        <v>487</v>
+      </c>
+      <c r="E62" s="30" t="s">
         <v>488</v>
       </c>
-      <c r="E62" s="30" t="s">
+      <c r="F62" s="30" t="s">
         <v>489</v>
-      </c>
-      <c r="F62" s="30" t="s">
-        <v>490</v>
       </c>
       <c r="G62" s="30" t="s">
         <v>147</v>
@@ -8727,13 +8709,13 @@
         <v>211</v>
       </c>
       <c r="D63" s="30" t="s">
+        <v>490</v>
+      </c>
+      <c r="E63" s="30" t="s">
         <v>491</v>
       </c>
-      <c r="E63" s="30" t="s">
+      <c r="F63" s="30" t="s">
         <v>492</v>
-      </c>
-      <c r="F63" s="30" t="s">
-        <v>493</v>
       </c>
       <c r="G63" s="30" t="s">
         <v>148</v>
@@ -8753,13 +8735,13 @@
         <v>205</v>
       </c>
       <c r="D64" s="30" t="s">
+        <v>493</v>
+      </c>
+      <c r="E64" s="30" t="s">
         <v>494</v>
       </c>
-      <c r="E64" s="30" t="s">
+      <c r="F64" s="30" t="s">
         <v>495</v>
-      </c>
-      <c r="F64" s="30" t="s">
-        <v>496</v>
       </c>
       <c r="G64" s="30" t="s">
         <v>147</v>
@@ -8779,13 +8761,13 @@
         <v>310</v>
       </c>
       <c r="D65" s="30" t="s">
+        <v>496</v>
+      </c>
+      <c r="E65" s="30" t="s">
         <v>497</v>
       </c>
-      <c r="E65" s="30" t="s">
+      <c r="F65" s="30" t="s">
         <v>498</v>
-      </c>
-      <c r="F65" s="30" t="s">
-        <v>499</v>
       </c>
       <c r="G65" s="30" t="s">
         <v>149</v>
@@ -8808,10 +8790,10 @@
         <v>197</v>
       </c>
       <c r="E66" s="30" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F66" s="30" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="G66" s="30" t="s">
         <v>148</v>
@@ -8834,10 +8816,10 @@
         <v>269</v>
       </c>
       <c r="E67" s="30" t="s">
+        <v>500</v>
+      </c>
+      <c r="F67" s="30" t="s">
         <v>501</v>
-      </c>
-      <c r="F67" s="30" t="s">
-        <v>502</v>
       </c>
       <c r="G67" s="30" t="s">
         <v>148</v>
@@ -8857,13 +8839,13 @@
         <v>301</v>
       </c>
       <c r="D68" s="30" t="s">
+        <v>502</v>
+      </c>
+      <c r="E68" s="30" t="s">
         <v>503</v>
       </c>
-      <c r="E68" s="30" t="s">
+      <c r="F68" s="30" t="s">
         <v>504</v>
-      </c>
-      <c r="F68" s="30" t="s">
-        <v>505</v>
       </c>
       <c r="G68" s="30" t="s">
         <v>149</v>
@@ -8886,10 +8868,10 @@
         <v>224</v>
       </c>
       <c r="E69" s="30" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F69" s="30" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G69" s="30" t="s">
         <v>147</v>
@@ -8912,10 +8894,10 @@
         <v>216</v>
       </c>
       <c r="E70" s="30" t="s">
+        <v>505</v>
+      </c>
+      <c r="F70" s="30" t="s">
         <v>506</v>
-      </c>
-      <c r="F70" s="30" t="s">
-        <v>507</v>
       </c>
       <c r="G70" s="30" t="s">
         <v>147</v>
@@ -8935,13 +8917,13 @@
         <v>229</v>
       </c>
       <c r="D71" s="30" t="s">
+        <v>507</v>
+      </c>
+      <c r="E71" s="30" t="s">
         <v>508</v>
       </c>
-      <c r="E71" s="30" t="s">
+      <c r="F71" s="30" t="s">
         <v>509</v>
-      </c>
-      <c r="F71" s="30" t="s">
-        <v>510</v>
       </c>
       <c r="G71" s="30" t="s">
         <v>149</v>
@@ -8961,13 +8943,13 @@
         <v>291</v>
       </c>
       <c r="D72" s="30" t="s">
+        <v>510</v>
+      </c>
+      <c r="E72" s="30" t="s">
         <v>511</v>
       </c>
-      <c r="E72" s="30" t="s">
+      <c r="F72" s="30" t="s">
         <v>512</v>
-      </c>
-      <c r="F72" s="30" t="s">
-        <v>513</v>
       </c>
       <c r="G72" s="30" t="s">
         <v>147</v>
@@ -8990,10 +8972,10 @@
         <v>199</v>
       </c>
       <c r="E73" s="30" t="s">
+        <v>513</v>
+      </c>
+      <c r="F73" s="30" t="s">
         <v>514</v>
-      </c>
-      <c r="F73" s="30" t="s">
-        <v>515</v>
       </c>
       <c r="G73" s="30" t="s">
         <v>148</v>
@@ -9013,13 +8995,13 @@
         <v>264</v>
       </c>
       <c r="D74" s="30" t="s">
+        <v>515</v>
+      </c>
+      <c r="E74" s="30" t="s">
         <v>516</v>
       </c>
-      <c r="E74" s="30" t="s">
+      <c r="F74" s="30" t="s">
         <v>517</v>
-      </c>
-      <c r="F74" s="30" t="s">
-        <v>518</v>
       </c>
       <c r="G74" s="30" t="s">
         <v>149</v>
@@ -9039,13 +9021,13 @@
         <v>292</v>
       </c>
       <c r="D75" s="30" t="s">
+        <v>518</v>
+      </c>
+      <c r="E75" s="30" t="s">
         <v>519</v>
       </c>
-      <c r="E75" s="30" t="s">
-        <v>520</v>
-      </c>
       <c r="F75" s="30" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G75" s="30" t="s">
         <v>149</v>
@@ -9065,13 +9047,13 @@
         <v>209</v>
       </c>
       <c r="D76" s="30" t="s">
+        <v>520</v>
+      </c>
+      <c r="E76" s="30" t="s">
         <v>521</v>
       </c>
-      <c r="E76" s="30" t="s">
-        <v>522</v>
-      </c>
       <c r="F76" s="30" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="G76" s="30" t="s">
         <v>149</v>
@@ -9094,10 +9076,10 @@
         <v>320</v>
       </c>
       <c r="E77" s="30" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F77" s="30" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="G77" s="30" t="s">
         <v>147</v>
@@ -9120,7 +9102,7 @@
         <v>256</v>
       </c>
       <c r="E78" s="30" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F78" s="30" t="s">
         <v>341</v>
@@ -9143,13 +9125,13 @@
         <v>277</v>
       </c>
       <c r="D79" s="30" t="s">
+        <v>523</v>
+      </c>
+      <c r="E79" s="30" t="s">
         <v>524</v>
       </c>
-      <c r="E79" s="30" t="s">
-        <v>525</v>
-      </c>
       <c r="F79" s="30" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="G79" s="30" t="s">
         <v>148</v>
@@ -9172,10 +9154,10 @@
         <v>240</v>
       </c>
       <c r="E80" s="30" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F80" s="30" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G80" s="30" t="s">
         <v>148</v>
@@ -9189,19 +9171,19 @@
         <v>77</v>
       </c>
       <c r="B81" s="21" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C81" s="26" t="s">
         <v>287</v>
       </c>
       <c r="D81" s="30" t="s">
+        <v>525</v>
+      </c>
+      <c r="E81" s="30" t="s">
         <v>526</v>
       </c>
-      <c r="E81" s="30" t="s">
+      <c r="F81" s="30" t="s">
         <v>527</v>
-      </c>
-      <c r="F81" s="30" t="s">
-        <v>528</v>
       </c>
       <c r="G81" s="30" t="s">
         <v>147</v>
@@ -9221,13 +9203,13 @@
         <v>179</v>
       </c>
       <c r="D82" s="30" t="s">
+        <v>528</v>
+      </c>
+      <c r="E82" s="30" t="s">
         <v>529</v>
       </c>
-      <c r="E82" s="30" t="s">
-        <v>530</v>
-      </c>
       <c r="F82" s="30" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="G82" s="30" t="s">
         <v>149</v>
@@ -9241,19 +9223,19 @@
         <v>129</v>
       </c>
       <c r="B83" s="21" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C83" s="26" t="s">
         <v>305</v>
       </c>
       <c r="D83" s="30" t="s">
+        <v>530</v>
+      </c>
+      <c r="E83" s="30" t="s">
         <v>531</v>
       </c>
-      <c r="E83" s="30" t="s">
+      <c r="F83" s="30" t="s">
         <v>532</v>
-      </c>
-      <c r="F83" s="30" t="s">
-        <v>533</v>
       </c>
       <c r="G83" s="30" t="s">
         <v>148</v>
@@ -9273,13 +9255,13 @@
         <v>243</v>
       </c>
       <c r="D84" s="30" t="s">
+        <v>533</v>
+      </c>
+      <c r="E84" s="30" t="s">
         <v>534</v>
       </c>
-      <c r="E84" s="30" t="s">
+      <c r="F84" s="30" t="s">
         <v>535</v>
-      </c>
-      <c r="F84" s="30" t="s">
-        <v>536</v>
       </c>
       <c r="G84" s="30" t="s">
         <v>150</v>
@@ -9293,19 +9275,19 @@
         <v>85</v>
       </c>
       <c r="B85" s="21" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C85" s="26" t="s">
         <v>321</v>
       </c>
       <c r="D85" s="30" t="s">
+        <v>536</v>
+      </c>
+      <c r="E85" s="30" t="s">
         <v>537</v>
       </c>
-      <c r="E85" s="30" t="s">
+      <c r="F85" s="30" t="s">
         <v>538</v>
-      </c>
-      <c r="F85" s="30" t="s">
-        <v>539</v>
       </c>
       <c r="G85" s="30" t="s">
         <v>149</v>
@@ -9319,19 +9301,19 @@
         <v>92</v>
       </c>
       <c r="B86" s="21" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C86" s="26" t="s">
         <v>316</v>
       </c>
       <c r="D86" s="30" t="s">
+        <v>539</v>
+      </c>
+      <c r="E86" s="30" t="s">
         <v>540</v>
       </c>
-      <c r="E86" s="30" t="s">
+      <c r="F86" s="30" t="s">
         <v>541</v>
-      </c>
-      <c r="F86" s="30" t="s">
-        <v>542</v>
       </c>
       <c r="G86" s="30" t="s">
         <v>149</v>
@@ -9351,13 +9333,13 @@
         <v>265</v>
       </c>
       <c r="D87" s="30" t="s">
+        <v>542</v>
+      </c>
+      <c r="E87" s="30" t="s">
         <v>543</v>
       </c>
-      <c r="E87" s="30" t="s">
+      <c r="F87" s="30" t="s">
         <v>544</v>
-      </c>
-      <c r="F87" s="30" t="s">
-        <v>545</v>
       </c>
       <c r="G87" s="30" t="s">
         <v>148</v>
@@ -9371,19 +9353,19 @@
         <v>67</v>
       </c>
       <c r="B88" s="21" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C88" s="26" t="s">
         <v>302</v>
       </c>
       <c r="D88" s="30" t="s">
+        <v>546</v>
+      </c>
+      <c r="E88" s="30" t="s">
         <v>547</v>
       </c>
-      <c r="E88" s="30" t="s">
+      <c r="F88" s="30" t="s">
         <v>548</v>
-      </c>
-      <c r="F88" s="30" t="s">
-        <v>549</v>
       </c>
       <c r="G88" s="30" t="s">
         <v>148</v>
@@ -9406,10 +9388,10 @@
         <v>190</v>
       </c>
       <c r="E89" s="30" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F89" s="30" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G89" s="30" t="s">
         <v>148</v>
@@ -9429,13 +9411,13 @@
         <v>186</v>
       </c>
       <c r="D90" s="30" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="E90" s="31" t="s">
         <v>346</v>
       </c>
       <c r="F90" s="30" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="G90" s="30" t="s">
         <v>148</v>
@@ -9458,10 +9440,10 @@
         <v>284</v>
       </c>
       <c r="E91" s="30" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="F91" s="30" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G91" s="30" t="s">
         <v>148</v>
@@ -9481,13 +9463,13 @@
         <v>181</v>
       </c>
       <c r="D92" s="30" t="s">
+        <v>553</v>
+      </c>
+      <c r="E92" s="30" t="s">
         <v>554</v>
       </c>
-      <c r="E92" s="30" t="s">
+      <c r="F92" s="30" t="s">
         <v>555</v>
-      </c>
-      <c r="F92" s="30" t="s">
-        <v>556</v>
       </c>
       <c r="G92" s="30" t="s">
         <v>148</v>
@@ -9501,19 +9483,19 @@
         <v>99</v>
       </c>
       <c r="B93" s="21" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C93" s="26" t="s">
         <v>276</v>
       </c>
       <c r="D93" s="30" t="s">
+        <v>556</v>
+      </c>
+      <c r="E93" s="30" t="s">
         <v>557</v>
       </c>
-      <c r="E93" s="30" t="s">
-        <v>558</v>
-      </c>
       <c r="F93" s="30" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="G93" s="30" t="s">
         <v>149</v>
@@ -9527,19 +9509,19 @@
         <v>103</v>
       </c>
       <c r="B94" s="21" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C94" s="26" t="s">
         <v>234</v>
       </c>
       <c r="D94" s="30" t="s">
+        <v>559</v>
+      </c>
+      <c r="E94" s="30" t="s">
         <v>560</v>
       </c>
-      <c r="E94" s="30" t="s">
-        <v>561</v>
-      </c>
       <c r="F94" s="30" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G94" s="30" t="s">
         <v>149</v>
@@ -9562,10 +9544,10 @@
         <v>202</v>
       </c>
       <c r="E95" s="30" t="s">
+        <v>561</v>
+      </c>
+      <c r="F95" s="30" t="s">
         <v>562</v>
-      </c>
-      <c r="F95" s="30" t="s">
-        <v>563</v>
       </c>
       <c r="G95" s="30" t="s">
         <v>148</v>
@@ -9588,10 +9570,10 @@
         <v>312</v>
       </c>
       <c r="E96" s="30" t="s">
+        <v>563</v>
+      </c>
+      <c r="F96" s="30" t="s">
         <v>564</v>
-      </c>
-      <c r="F96" s="30" t="s">
-        <v>565</v>
       </c>
       <c r="G96" s="30" t="s">
         <v>147</v>
@@ -9605,19 +9587,19 @@
         <v>111</v>
       </c>
       <c r="B97" s="21" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C97" s="26" t="s">
         <v>248</v>
       </c>
       <c r="D97" s="30" t="s">
+        <v>565</v>
+      </c>
+      <c r="E97" s="30" t="s">
         <v>566</v>
       </c>
-      <c r="E97" s="30" t="s">
+      <c r="F97" s="30" t="s">
         <v>567</v>
-      </c>
-      <c r="F97" s="30" t="s">
-        <v>568</v>
       </c>
       <c r="G97" s="30" t="s">
         <v>148</v>
@@ -9637,13 +9619,13 @@
         <v>247</v>
       </c>
       <c r="D98" s="30" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="E98" s="30" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F98" s="30" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G98" s="30" t="s">
         <v>147</v>
@@ -9663,13 +9645,13 @@
         <v>297</v>
       </c>
       <c r="D99" s="30" t="s">
+        <v>569</v>
+      </c>
+      <c r="E99" s="30" t="s">
         <v>570</v>
       </c>
-      <c r="E99" s="30" t="s">
+      <c r="F99" s="30" t="s">
         <v>571</v>
-      </c>
-      <c r="F99" s="30" t="s">
-        <v>572</v>
       </c>
       <c r="G99" s="30" t="s">
         <v>147</v>
@@ -9689,13 +9671,13 @@
         <v>210</v>
       </c>
       <c r="D100" s="30" t="s">
+        <v>572</v>
+      </c>
+      <c r="E100" s="30" t="s">
         <v>573</v>
       </c>
-      <c r="E100" s="30" t="s">
-        <v>574</v>
-      </c>
       <c r="F100" s="30" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G100" s="30" t="s">
         <v>149</v>
@@ -9706,7 +9688,7 @@
     </row>
     <row r="101" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A101" s="21" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B101" s="21" t="s">
         <v>332</v>
@@ -9715,13 +9697,13 @@
         <v>221</v>
       </c>
       <c r="D101" s="30" t="s">
+        <v>575</v>
+      </c>
+      <c r="E101" s="30" t="s">
         <v>576</v>
       </c>
-      <c r="E101" s="30" t="s">
+      <c r="F101" s="30" t="s">
         <v>577</v>
-      </c>
-      <c r="F101" s="30" t="s">
-        <v>578</v>
       </c>
       <c r="G101" s="30" t="s">
         <v>148</v>
@@ -9741,13 +9723,13 @@
         <v>241</v>
       </c>
       <c r="D102" s="30" t="s">
+        <v>578</v>
+      </c>
+      <c r="E102" s="30" t="s">
         <v>579</v>
       </c>
-      <c r="E102" s="30" t="s">
+      <c r="F102" s="30" t="s">
         <v>580</v>
-      </c>
-      <c r="F102" s="30" t="s">
-        <v>581</v>
       </c>
       <c r="G102" s="30" t="s">
         <v>147</v>
@@ -9770,10 +9752,10 @@
         <v>231</v>
       </c>
       <c r="E103" s="30" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="F103" s="30" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="G103" s="30" t="s">
         <v>147</v>
@@ -9796,10 +9778,10 @@
         <v>193</v>
       </c>
       <c r="E104" s="30" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="F104" s="30" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G104" s="30" t="s">
         <v>147</v>
@@ -9819,13 +9801,13 @@
         <v>222</v>
       </c>
       <c r="D105" s="30" t="s">
+        <v>583</v>
+      </c>
+      <c r="E105" s="30" t="s">
         <v>584</v>
       </c>
-      <c r="E105" s="30" t="s">
+      <c r="F105" s="30" t="s">
         <v>585</v>
-      </c>
-      <c r="F105" s="30" t="s">
-        <v>586</v>
       </c>
       <c r="G105" s="30" t="s">
         <v>148</v>
@@ -9848,10 +9830,10 @@
         <v>260</v>
       </c>
       <c r="E106" s="30" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F106" s="30" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="G106" s="30" t="s">
         <v>149</v>
@@ -9874,10 +9856,10 @@
         <v>207</v>
       </c>
       <c r="E107" s="30" t="s">
+        <v>587</v>
+      </c>
+      <c r="F107" s="30" t="s">
         <v>588</v>
-      </c>
-      <c r="F107" s="30" t="s">
-        <v>589</v>
       </c>
       <c r="G107" s="30" t="s">
         <v>148</v>
@@ -9897,13 +9879,13 @@
         <v>290</v>
       </c>
       <c r="D108" s="30" t="s">
+        <v>589</v>
+      </c>
+      <c r="E108" s="30" t="s">
         <v>590</v>
       </c>
-      <c r="E108" s="30" t="s">
-        <v>591</v>
-      </c>
       <c r="F108" s="30" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G108" s="30" t="s">
         <v>148</v>
@@ -9923,13 +9905,13 @@
         <v>273</v>
       </c>
       <c r="D109" s="30" t="s">
+        <v>591</v>
+      </c>
+      <c r="E109" s="30" t="s">
+        <v>390</v>
+      </c>
+      <c r="F109" s="30" t="s">
         <v>592</v>
-      </c>
-      <c r="E109" s="30" t="s">
-        <v>391</v>
-      </c>
-      <c r="F109" s="30" t="s">
-        <v>593</v>
       </c>
       <c r="G109" s="30" t="s">
         <v>147</v>
@@ -9949,13 +9931,13 @@
         <v>208</v>
       </c>
       <c r="D110" s="30" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="E110" s="30" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F110" s="30" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G110" s="30" t="s">
         <v>148</v>
@@ -9975,13 +9957,13 @@
         <v>171</v>
       </c>
       <c r="D111" s="31" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="E111" s="31" t="s">
         <v>346</v>
       </c>
       <c r="F111" s="31" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G111" s="30" t="s">
         <v>147</v>
@@ -10004,10 +9986,10 @@
         <v>271</v>
       </c>
       <c r="E112" s="30" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="F112" s="30" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="G112" s="30" t="s">
         <v>148</v>
@@ -10021,19 +10003,19 @@
         <v>106</v>
       </c>
       <c r="B113" s="21" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C113" s="26" t="s">
         <v>261</v>
       </c>
       <c r="D113" s="30" t="s">
+        <v>597</v>
+      </c>
+      <c r="E113" s="30" t="s">
         <v>598</v>
       </c>
-      <c r="E113" s="30" t="s">
+      <c r="F113" s="30" t="s">
         <v>599</v>
-      </c>
-      <c r="F113" s="30" t="s">
-        <v>600</v>
       </c>
       <c r="G113" s="30" t="s">
         <v>148</v>
@@ -10053,13 +10035,13 @@
         <v>295</v>
       </c>
       <c r="D114" s="30" t="s">
+        <v>600</v>
+      </c>
+      <c r="E114" s="30" t="s">
         <v>601</v>
       </c>
-      <c r="E114" s="30" t="s">
-        <v>602</v>
-      </c>
       <c r="F114" s="30" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G114" s="30" t="s">
         <v>147</v>
@@ -10079,10 +10061,10 @@
         <v>309</v>
       </c>
       <c r="D115" s="30" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E115" s="30" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F115" s="30" t="s">
         <v>147</v>
@@ -10108,10 +10090,10 @@
         <v>250</v>
       </c>
       <c r="E116" s="30" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F116" s="30" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G116" s="30" t="s">
         <v>149</v>
@@ -10134,10 +10116,10 @@
         <v>299</v>
       </c>
       <c r="E117" s="30" t="s">
+        <v>604</v>
+      </c>
+      <c r="F117" s="30" t="s">
         <v>605</v>
-      </c>
-      <c r="F117" s="30" t="s">
-        <v>606</v>
       </c>
       <c r="G117" s="30" t="s">
         <v>148</v>
@@ -10157,13 +10139,13 @@
         <v>296</v>
       </c>
       <c r="D118" s="30" t="s">
+        <v>606</v>
+      </c>
+      <c r="E118" s="30" t="s">
         <v>607</v>
       </c>
-      <c r="E118" s="30" t="s">
+      <c r="F118" s="30" t="s">
         <v>608</v>
-      </c>
-      <c r="F118" s="30" t="s">
-        <v>609</v>
       </c>
       <c r="G118" s="30" t="s">
         <v>148</v>
@@ -10183,13 +10165,13 @@
         <v>266</v>
       </c>
       <c r="D119" s="30" t="s">
+        <v>609</v>
+      </c>
+      <c r="E119" s="30" t="s">
         <v>610</v>
       </c>
-      <c r="E119" s="30" t="s">
+      <c r="F119" s="30" t="s">
         <v>611</v>
-      </c>
-      <c r="F119" s="30" t="s">
-        <v>612</v>
       </c>
       <c r="G119" s="30" t="s">
         <v>148</v>
@@ -10209,13 +10191,13 @@
         <v>225</v>
       </c>
       <c r="D120" s="30" t="s">
+        <v>612</v>
+      </c>
+      <c r="E120" s="30" t="s">
         <v>613</v>
       </c>
-      <c r="E120" s="30" t="s">
+      <c r="F120" s="30" t="s">
         <v>614</v>
-      </c>
-      <c r="F120" s="30" t="s">
-        <v>615</v>
       </c>
       <c r="G120" s="30" t="s">
         <v>148</v>
@@ -10235,13 +10217,13 @@
         <v>275</v>
       </c>
       <c r="D121" s="30" t="s">
+        <v>615</v>
+      </c>
+      <c r="E121" s="30" t="s">
         <v>616</v>
       </c>
-      <c r="E121" s="30" t="s">
+      <c r="F121" s="30" t="s">
         <v>617</v>
-      </c>
-      <c r="F121" s="30" t="s">
-        <v>618</v>
       </c>
       <c r="G121" s="30" t="s">
         <v>147</v>
@@ -10255,19 +10237,19 @@
         <v>116</v>
       </c>
       <c r="B122" s="21" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C122" s="26" t="s">
         <v>200</v>
       </c>
       <c r="D122" s="30" t="s">
+        <v>618</v>
+      </c>
+      <c r="E122" s="30" t="s">
         <v>619</v>
       </c>
-      <c r="E122" s="30" t="s">
+      <c r="F122" s="30" t="s">
         <v>620</v>
-      </c>
-      <c r="F122" s="30" t="s">
-        <v>621</v>
       </c>
       <c r="G122" s="30" t="s">
         <v>148</v>
@@ -10290,7 +10272,7 @@
         <v>168</v>
       </c>
       <c r="E123" s="30" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="F123" s="30" t="s">
         <v>338</v>
@@ -10313,13 +10295,13 @@
         <v>330</v>
       </c>
       <c r="D124" s="31" t="s">
+        <v>625</v>
+      </c>
+      <c r="E124" s="31" t="s">
         <v>626</v>
       </c>
-      <c r="E124" s="31" t="s">
+      <c r="F124" s="31" t="s">
         <v>627</v>
-      </c>
-      <c r="F124" s="31" t="s">
-        <v>628</v>
       </c>
       <c r="G124" s="30" t="s">
         <v>149</v>
@@ -10339,13 +10321,13 @@
         <v>331</v>
       </c>
       <c r="D125" s="31" t="s">
+        <v>628</v>
+      </c>
+      <c r="E125" s="33" t="s">
         <v>629</v>
       </c>
-      <c r="E125" s="33" t="s">
-        <v>630</v>
-      </c>
       <c r="F125" s="32" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G125" s="30" t="s">
         <v>148</v>
@@ -10365,13 +10347,13 @@
         <v>221</v>
       </c>
       <c r="D126" s="31" t="s">
+        <v>630</v>
+      </c>
+      <c r="E126" s="31" t="s">
         <v>631</v>
       </c>
-      <c r="E126" s="31" t="s">
+      <c r="F126" s="31" t="s">
         <v>632</v>
-      </c>
-      <c r="F126" s="31" t="s">
-        <v>633</v>
       </c>
       <c r="G126" s="30" t="s">
         <v>147</v>
@@ -10391,13 +10373,13 @@
         <v>327</v>
       </c>
       <c r="D127" s="31" t="s">
+        <v>633</v>
+      </c>
+      <c r="E127" s="35" t="s">
+        <v>644</v>
+      </c>
+      <c r="F127" s="31" t="s">
         <v>634</v>
-      </c>
-      <c r="E127" s="35" t="s">
-        <v>645</v>
-      </c>
-      <c r="F127" s="31" t="s">
-        <v>635</v>
       </c>
       <c r="G127" s="30" t="s">
         <v>150</v>
@@ -10417,13 +10399,13 @@
         <v>329</v>
       </c>
       <c r="D128" s="31" t="s">
+        <v>635</v>
+      </c>
+      <c r="E128" s="35" t="s">
         <v>636</v>
       </c>
-      <c r="E128" s="35" t="s">
+      <c r="F128" s="31" t="s">
         <v>637</v>
-      </c>
-      <c r="F128" s="31" t="s">
-        <v>638</v>
       </c>
       <c r="G128" s="30" t="s">
         <v>147</v>
@@ -10443,13 +10425,13 @@
         <v>325</v>
       </c>
       <c r="D129" s="31" t="s">
+        <v>638</v>
+      </c>
+      <c r="E129" s="34" t="s">
         <v>639</v>
       </c>
-      <c r="E129" s="34" t="s">
+      <c r="F129" s="31" t="s">
         <v>640</v>
-      </c>
-      <c r="F129" s="31" t="s">
-        <v>641</v>
       </c>
       <c r="G129" s="30" t="s">
         <v>147</v>
@@ -10469,13 +10451,13 @@
         <v>324</v>
       </c>
       <c r="D130" s="31" t="s">
+        <v>641</v>
+      </c>
+      <c r="E130" s="37" t="s">
         <v>642</v>
       </c>
-      <c r="E130" s="37" t="s">
+      <c r="F130" s="36" t="s">
         <v>643</v>
-      </c>
-      <c r="F130" s="36" t="s">
-        <v>644</v>
       </c>
       <c r="G130" s="30" t="s">
         <v>149</v>
@@ -10495,13 +10477,13 @@
         <v>328</v>
       </c>
       <c r="D131" s="31" t="s">
+        <v>645</v>
+      </c>
+      <c r="E131" s="31" t="s">
         <v>646</v>
       </c>
-      <c r="E131" s="31" t="s">
+      <c r="F131" s="31" t="s">
         <v>647</v>
-      </c>
-      <c r="F131" s="31" t="s">
-        <v>648</v>
       </c>
       <c r="G131" s="30" t="s">
         <v>149</v>
@@ -10512,22 +10494,22 @@
     </row>
     <row r="132" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A132" s="23" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B132" s="23" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C132" s="31" t="s">
         <v>326</v>
       </c>
       <c r="D132" s="38" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="E132" s="35" t="s">
+        <v>649</v>
+      </c>
+      <c r="F132" s="39" t="s">
         <v>650</v>
-      </c>
-      <c r="F132" s="39" t="s">
-        <v>651</v>
       </c>
       <c r="G132" s="30" t="s">
         <v>150</v>
@@ -10541,19 +10523,19 @@
         <v>16</v>
       </c>
       <c r="B133" s="23" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="C133" s="31" t="s">
         <v>323</v>
       </c>
       <c r="D133" s="31" t="s">
+        <v>652</v>
+      </c>
+      <c r="E133" s="31" t="s">
         <v>653</v>
       </c>
-      <c r="E133" s="31" t="s">
+      <c r="F133" s="31" t="s">
         <v>654</v>
-      </c>
-      <c r="F133" s="31" t="s">
-        <v>655</v>
       </c>
       <c r="G133" s="30" t="s">
         <v>148</v>
@@ -10570,16 +10552,16 @@
         <v>7</v>
       </c>
       <c r="C134" s="31" t="s">
+        <v>656</v>
+      </c>
+      <c r="D134" s="31" t="s">
         <v>657</v>
       </c>
-      <c r="D134" s="31" t="s">
+      <c r="E134" s="31" t="s">
         <v>658</v>
       </c>
-      <c r="E134" s="31" t="s">
+      <c r="F134" s="31" t="s">
         <v>659</v>
-      </c>
-      <c r="F134" s="31" t="s">
-        <v>660</v>
       </c>
       <c r="G134" s="30" t="s">
         <v>148</v>
@@ -10596,16 +10578,16 @@
         <v>9</v>
       </c>
       <c r="C135" s="31" t="s">
+        <v>660</v>
+      </c>
+      <c r="D135" s="36" t="s">
+        <v>663</v>
+      </c>
+      <c r="E135" s="37" t="s">
         <v>661</v>
       </c>
-      <c r="D135" s="36" t="s">
-        <v>664</v>
-      </c>
-      <c r="E135" s="37" t="s">
+      <c r="F135" s="36" t="s">
         <v>662</v>
-      </c>
-      <c r="F135" s="36" t="s">
-        <v>663</v>
       </c>
       <c r="G135" s="30" t="s">
         <v>147</v>
@@ -10700,9 +10682,9 @@
     <col min="11" max="11" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B1" s="41" t="s">
         <v>0</v>
@@ -10737,7 +10719,7 @@
     </row>
     <row r="2" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="42" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B2" s="43">
         <v>0.4</v>
@@ -10772,7 +10754,7 @@
     </row>
     <row r="3" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="42" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B3" s="43">
         <v>1</v>
@@ -10807,7 +10789,7 @@
     </row>
     <row r="4" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="42" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B4" s="43">
         <v>1.5</v>
@@ -10842,7 +10824,7 @@
     </row>
     <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="42" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B5" s="43">
         <v>2</v>
@@ -10877,7 +10859,7 @@
     </row>
     <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="42" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B6" s="43">
         <v>2.5</v>
@@ -10912,7 +10894,7 @@
     </row>
     <row r="7" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="42" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B7" s="43">
         <v>2.75</v>
@@ -10947,7 +10929,7 @@
     </row>
     <row r="8" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="42" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B8" s="43">
         <v>4</v>
@@ -10982,7 +10964,7 @@
     </row>
     <row r="9" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="42" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B9" s="43">
         <v>4</v>

</xml_diff>